<commit_message>
fixed download button and added email preview
</commit_message>
<xml_diff>
--- a/updated.xlsx
+++ b/updated.xlsx
@@ -4,13 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mastersheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Branch with Emails" sheetId="2" r:id="rId2"/>
+    <sheet name="Recording" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,8 +348,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>